<commit_message>
MInor changes in BDA
</commit_message>
<xml_diff>
--- a/4.6_Building_Defensive_Alliance_Latest/performance_check/file_type_performance_check_BDA.xlsx
+++ b/4.6_Building_Defensive_Alliance_Latest/performance_check/file_type_performance_check_BDA.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1109,9 +1109,152 @@
         <v>8</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>8.414351851851851e-09</v>
+        <v>1.157407407407407e-08</v>
       </c>
       <c r="C53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>8</v>
+      </c>
+      <c r="B54" s="1" t="n">
+        <v>3.472222222222222e-08</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>8</v>
+      </c>
+      <c r="B55" s="1" t="n">
+        <v>1.157407407407407e-08</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>8</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <v>2.314814814814815e-08</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>8</v>
+      </c>
+      <c r="B57" s="1" t="n">
+        <v>2.314814814814815e-08</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>7</v>
+      </c>
+      <c r="B58" s="1" t="n">
+        <v>1.157407407407407e-08</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>7</v>
+      </c>
+      <c r="B59" s="1" t="n">
+        <v>7.638888888888889e-07</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>8</v>
+      </c>
+      <c r="B60" s="1" t="n">
+        <v>2.314814814814815e-08</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>8</v>
+      </c>
+      <c r="B61" s="1" t="n">
+        <v>2.314814814814815e-08</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>8</v>
+      </c>
+      <c r="B62" s="1" t="n">
+        <v>1.157407407407407e-08</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>8</v>
+      </c>
+      <c r="B63" s="1" t="n">
+        <v>8.564814814814814e-07</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>8</v>
+      </c>
+      <c r="B64" s="1" t="n">
+        <v>2.297453703703704e-08</v>
+      </c>
+      <c r="C64" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>